<commit_message>
data collection tutorial updated
</commit_message>
<xml_diff>
--- a/GitHubPages/documents/StationFwdtrace_request_Frozen Fruit Sales_725897958_all.xlsx
+++ b/GitHubPages/documents/StationFwdtrace_request_Frozen Fruit Sales_725897958_all.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Production - Fwdtrace" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Production - Fwdtrace'!$A$1:$N$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Production - Fwdtrace'!$A$1:$N$46</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="71">
   <si>
     <t>EAN</t>
   </si>
@@ -290,25 +290,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -764,7 +752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1167,32 +1155,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1263,17 +1225,6 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1358,452 +1309,412 @@
   </borders>
   <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="38" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="38" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="37" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="37" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="37" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2223,1381 +2134,1258 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="12.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4.42578125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.7109375" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.28515625" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="34.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.140625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="15" max="19" width="11.42578125" style="14" collapsed="1"/>
-    <col min="20" max="16384" width="11.42578125" style="15" collapsed="1"/>
+    <col min="1" max="1" width="16.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="12.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12" style="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="4.42578125" style="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.7109375" style="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.28515625" style="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="15" max="19" width="11.42578125" style="12" collapsed="1"/>
+    <col min="20" max="16384" width="11.42578125" style="13" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="87" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="89"/>
-      <c r="I1" s="80" t="s">
+      <c r="H1" s="52"/>
+      <c r="I1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-    </row>
-    <row r="3" spans="1:19" s="17" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:19" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
     </row>
     <row r="4" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="86" t="s">
+      <c r="E4" s="44"/>
+      <c r="F4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="83" t="s">
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="62" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="64"/>
-      <c r="B5" s="70" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="70" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="85" t="s">
+      <c r="J5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="85" t="s">
+      <c r="K5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="85" t="s">
+      <c r="L5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="78" t="s">
+      <c r="M5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="62"/>
-      <c r="O5" s="16"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="69"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="4" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="70"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="16"/>
-    </row>
-    <row r="7" spans="1:19" s="17" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="I6" s="44"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" s="15" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="20" t="s">
+      <c r="E7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="N7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
     </row>
     <row r="8" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="20" t="s">
+      <c r="E8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="16"/>
+      <c r="N8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="22" t="s">
+      <c r="M9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="16"/>
+      <c r="N9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="16"/>
-    </row>
-    <row r="11" spans="1:19" s="25" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-    </row>
-    <row r="12" spans="1:19" s="25" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+    </row>
+    <row r="12" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-    </row>
-    <row r="13" spans="1:19" s="25" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+    </row>
+    <row r="13" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-    </row>
-    <row r="14" spans="1:19" s="25" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+    </row>
+    <row r="14" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-    </row>
-    <row r="15" spans="1:19" s="25" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+    </row>
+    <row r="15" spans="1:19" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
     </row>
     <row r="16" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="16"/>
-    </row>
-    <row r="17" spans="1:19" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="14"/>
+    </row>
+    <row r="17" spans="1:19" s="26" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="68" t="s">
+      <c r="E17" s="60"/>
+      <c r="F17" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="71" t="s">
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="62" t="s">
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="26"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-    </row>
-    <row r="18" spans="1:19" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
-      <c r="B18" s="54" t="s">
+      <c r="O17" s="24"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+    </row>
+    <row r="18" spans="1:19" s="26" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57"/>
+      <c r="B18" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="54" t="s">
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="66" t="s">
+      <c r="J18" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="66" t="s">
+      <c r="K18" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="66" t="s">
+      <c r="L18" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="52" t="s">
+      <c r="M18" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="N18" s="62"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-    </row>
-    <row r="19" spans="1:19" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="2" t="s">
+      <c r="N18" s="59"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+    </row>
+    <row r="19" spans="1:19" s="26" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="76"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="55"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
     </row>
     <row r="20" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="30" t="s">
+      <c r="E20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="I20" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="29" t="s">
+      <c r="K20" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="L20" s="29" t="s">
+      <c r="L20" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N20" s="31" t="s">
+      <c r="N20" s="16" t="s">
         <v>32</v>
       </c>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N21" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="N21" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O22"/>
+      <c r="N22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="33" t="s">
+      <c r="C23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="34" t="s">
+      <c r="E23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="35" t="s">
+      <c r="J23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="K23" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L23" s="35" t="s">
+      <c r="L23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="36" t="s">
+      <c r="M23" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="16" t="s">
         <v>32</v>
       </c>
       <c r="O23" s="16"/>
     </row>
-    <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N24" t="s">
-        <v>32</v>
-      </c>
-      <c r="O24"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="N24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N25" t="s">
-        <v>32</v>
-      </c>
-      <c r="O25"/>
+      <c r="N25" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
-      <c r="B26" s="33" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="33" t="s">
+      <c r="C26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="33" t="s">
+      <c r="E26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="35" t="s">
+      <c r="J26" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K26" s="35" t="s">
+      <c r="K26" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="L26" s="35" t="s">
+      <c r="L26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M26" s="36" t="s">
+      <c r="M26" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N26" s="37" t="s">
+      <c r="N26" s="16" t="s">
         <v>32</v>
       </c>
       <c r="O26" s="16"/>
     </row>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="47" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27" s="32"/>
+      <c r="B27" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="47" t="s">
+      <c r="C27" s="27"/>
+      <c r="D27" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34">
+      <c r="E27" s="27"/>
+      <c r="F27" s="28">
         <v>28</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="28">
         <v>8</v>
       </c>
-      <c r="H27" s="34">
+      <c r="H27" s="28">
         <v>2014</v>
       </c>
-      <c r="I27" s="47" t="s">
+      <c r="I27" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="J27" s="48" t="s">
+      <c r="J27" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="48" t="s">
+      <c r="K27" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="48" t="s">
+      <c r="L27" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="M27" s="49" t="s">
+      <c r="M27" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="N27" s="37"/>
-      <c r="O27" s="16"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="14"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34">
-        <v>28</v>
-      </c>
-      <c r="G28" s="34">
-        <v>8</v>
-      </c>
-      <c r="H28" s="34">
-        <v>2014</v>
-      </c>
-      <c r="I28" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="J28" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="L28" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="M28" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="N28" s="37"/>
-      <c r="O28" s="16"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="14"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34">
-        <v>28</v>
-      </c>
-      <c r="G29" s="34">
-        <v>8</v>
-      </c>
-      <c r="H29" s="34">
-        <v>2014</v>
-      </c>
-      <c r="I29" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="J29" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="K29" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="L29" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="M29" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="N29" s="37"/>
-      <c r="O29" s="16"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="14"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="16"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="14"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="16"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="14"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="38"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="16"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="14"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="38"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="16"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="14"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="38"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="16"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="14"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="16"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="14"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="38"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="16"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="14"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="38"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="16"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="14"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="38"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="16"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="14"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="38"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="16"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="14"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="38"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="16"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="14"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="38"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="16"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="14"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="38"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="37"/>
-      <c r="O42" s="16"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="14"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="38"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="37"/>
-      <c r="O43" s="16"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="30"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="14"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="38"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="37"/>
-      <c r="O44" s="16"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="30"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="14"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="38"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="37"/>
-      <c r="O45" s="16"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="38"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="37"/>
-      <c r="O46" s="16"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="38"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="35"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="37"/>
-      <c r="O47" s="16"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="38"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="36"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="16"/>
-    </row>
-    <row r="49" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="40"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="16"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="14"/>
+    </row>
+    <row r="46" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="33"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A16:N16"/>
-    <mergeCell ref="A15:N15"/>
-    <mergeCell ref="M5:M6"/>
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="A11:N11"/>
@@ -3614,6 +3402,32 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:N3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7 F13 F2:F3 F17:F1048576">

</xml_diff>